<commit_message>
Fixed some BoM formatting issues
</commit_message>
<xml_diff>
--- a/amproc/BoM fm row.xlsx
+++ b/amproc/BoM fm row.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tom\Documents\Electronics\amtx\Audio\amproc\amproc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A620C5A3-C7B5-4517-965A-8807A9891444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73689CE6-DFAC-428E-8CCF-2DC463541A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="7275" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,8 +884,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.0000_-;\-&quot;£&quot;* #,##0.0000_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1365,14 +1366,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="8"/>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1743,8 +1743,9 @@
     <col min="5" max="5" width="33.765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.4609375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.53515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.23046875" style="2"/>
+    <col min="9" max="9" width="23.53515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.3046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.61328125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1776,17 +1777,17 @@
       <c r="I1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>73</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>285</v>
       </c>
@@ -1811,19 +1812,18 @@
       <c r="H2" t="s">
         <v>79</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>2860078</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="4">
         <v>7.1300000000000002E-2</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="4">
         <f>B2*J2</f>
         <v>0.1426</v>
       </c>
-      <c r="L2"/>
-    </row>
-    <row r="3" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>233</v>
       </c>
@@ -1851,16 +1851,15 @@
       <c r="I3" t="s">
         <v>244</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="4">
         <v>0.187</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="4">
         <f t="shared" ref="K3:K36" si="0">B3*J3</f>
         <v>0.374</v>
       </c>
-      <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>255</v>
       </c>
@@ -1888,16 +1887,15 @@
       <c r="I4" t="s">
         <v>247</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>0.24399999999999999</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <f t="shared" si="0"/>
         <v>0.48799999999999999</v>
       </c>
-      <c r="L4"/>
-    </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1925,16 +1923,15 @@
       <c r="I5" t="s">
         <v>86</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="4">
         <v>0.439</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="4">
         <f t="shared" si="0"/>
         <v>0.878</v>
       </c>
-      <c r="L5"/>
-    </row>
-    <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -1962,16 +1959,15 @@
       <c r="I6" t="s">
         <v>82</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="4">
         <v>8.2299999999999998E-2</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="4">
         <f t="shared" si="0"/>
         <v>0.57609999999999995</v>
       </c>
-      <c r="L6"/>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -1999,16 +1995,15 @@
       <c r="I7" t="s">
         <v>92</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="4">
         <v>0.128</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
         <v>0.25600000000000001</v>
       </c>
-      <c r="L7"/>
-    </row>
-    <row r="8" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2036,16 +2031,15 @@
       <c r="I8" t="s">
         <v>95</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="4">
         <v>0.13700000000000001</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
         <v>0.13700000000000001</v>
       </c>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -2073,16 +2067,15 @@
       <c r="I9" t="s">
         <v>89</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="4">
         <v>7.4499999999999997E-2</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="4">
         <f t="shared" si="0"/>
         <v>0.44699999999999995</v>
       </c>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2110,16 +2103,15 @@
       <c r="I10" t="s">
         <v>98</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="4">
         <v>0.13</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>254</v>
       </c>
@@ -2147,16 +2139,15 @@
       <c r="I11" t="s">
         <v>262</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="4">
         <f t="shared" si="0"/>
         <v>0.13500000000000001</v>
       </c>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2184,16 +2175,15 @@
       <c r="I12" t="s">
         <v>101</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="4">
         <v>0.27500000000000002</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2221,16 +2211,15 @@
       <c r="I13" t="s">
         <v>106</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="4">
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
         <v>6.0900000000000003E-2</v>
       </c>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2258,16 +2247,15 @@
       <c r="I14" t="s">
         <v>110</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="4">
         <v>3.1899999999999998E-2</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
         <v>0.19139999999999999</v>
       </c>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2295,23 +2283,21 @@
       <c r="I15" t="s">
         <v>115</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="4">
         <v>0.193</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
         <v>1.1579999999999999</v>
       </c>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>120</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16"/>
       <c r="D16" t="s">
         <v>116</v>
       </c>
@@ -2330,16 +2316,15 @@
       <c r="I16" t="s">
         <v>119</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="4">
         <v>0.59</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
         <v>1.77</v>
       </c>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2367,10 +2352,10 @@
       <c r="I17" t="s">
         <v>124</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="4">
         <v>0.58099999999999996</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
         <v>0.58099999999999996</v>
       </c>
@@ -2378,7 +2363,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2406,10 +2391,10 @@
       <c r="I18" t="s">
         <v>131</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="4">
         <v>0.247</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="4">
         <f t="shared" si="0"/>
         <v>0.247</v>
       </c>
@@ -2417,7 +2402,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2445,10 +2430,10 @@
       <c r="I19" t="s">
         <v>135</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="4">
         <v>0.13200000000000001</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>0.13200000000000001</v>
       </c>
@@ -2456,7 +2441,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2484,10 +2469,10 @@
       <c r="I20" t="s">
         <v>141</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="4">
         <v>2.52E-2</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="4">
         <f t="shared" si="0"/>
         <v>2.52E-2</v>
       </c>
@@ -2495,7 +2480,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>279</v>
       </c>
@@ -2523,16 +2508,15 @@
       <c r="I21" t="s">
         <v>284</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="4">
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
         <v>0.185</v>
       </c>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2560,16 +2544,15 @@
       <c r="I22" t="s">
         <v>147</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="4">
         <v>0.151</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
         <v>0.45299999999999996</v>
       </c>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -2597,16 +2580,15 @@
       <c r="I23" t="s">
         <v>149</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="4">
         <v>0.16400000000000001</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
         <v>0.98399999999999999</v>
       </c>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2634,16 +2616,15 @@
       <c r="I24" t="s">
         <v>153</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="4">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
         <v>5.7599999999999998E-2</v>
       </c>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>230</v>
       </c>
@@ -2671,16 +2652,15 @@
       <c r="I25" t="s">
         <v>266</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="4">
         <v>2.98E-2</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="4">
         <f t="shared" si="0"/>
         <v>2.98E-2</v>
       </c>
-      <c r="L25"/>
-    </row>
-    <row r="26" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2708,16 +2688,15 @@
       <c r="I26" t="s">
         <v>157</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="4">
         <v>2.8400000000000002E-2</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="4">
         <f t="shared" si="0"/>
         <v>5.6800000000000003E-2</v>
       </c>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2745,16 +2724,15 @@
       <c r="I27" t="s">
         <v>167</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="4">
         <v>0.03</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="4">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>232</v>
       </c>
@@ -2782,16 +2760,15 @@
       <c r="I28" t="s">
         <v>271</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="4">
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="4">
         <f t="shared" si="0"/>
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>231</v>
       </c>
@@ -2819,16 +2796,15 @@
       <c r="I29" t="s">
         <v>270</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="4">
         <v>3.0700000000000002E-2</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="4">
         <f t="shared" si="0"/>
         <v>3.0700000000000002E-2</v>
       </c>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2856,16 +2832,15 @@
       <c r="I30" t="s">
         <v>169</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="4">
         <v>2.86E-2</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="4">
         <f t="shared" si="0"/>
         <v>2.86E-2</v>
       </c>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2893,16 +2868,15 @@
       <c r="I31" t="s">
         <v>170</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="4">
         <v>0.03</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="4">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
-      <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2930,16 +2904,15 @@
       <c r="I32" t="s">
         <v>173</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="4">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="4">
         <f t="shared" si="0"/>
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="L32"/>
-    </row>
-    <row r="33" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>234</v>
       </c>
@@ -2967,16 +2940,15 @@
       <c r="I33" t="s">
         <v>250</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="4">
         <v>2.9499999999999998E-2</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="4">
         <f t="shared" si="0"/>
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="L33"/>
-    </row>
-    <row r="34" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>235</v>
       </c>
@@ -3004,16 +2976,15 @@
       <c r="I34" t="s">
         <v>253</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="4">
         <v>2.8199999999999999E-2</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="4">
         <f t="shared" si="0"/>
         <v>5.6399999999999999E-2</v>
       </c>
-      <c r="L34"/>
-    </row>
-    <row r="35" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>177</v>
       </c>
@@ -3041,16 +3012,15 @@
       <c r="I35" t="s">
         <v>176</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="4">
         <v>0.03</v>
       </c>
-      <c r="K35">
+      <c r="K35" s="4">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="L35"/>
-    </row>
-    <row r="36" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -3078,16 +3048,15 @@
       <c r="I36" t="s">
         <v>179</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="4">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="4">
         <f t="shared" si="0"/>
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="L36"/>
-    </row>
-    <row r="37" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -3115,16 +3084,15 @@
       <c r="I37" t="s">
         <v>185</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="4">
         <v>7.8600000000000003E-2</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="4">
         <f t="shared" ref="K37:K50" si="1">B37*J37</f>
         <v>0.15720000000000001</v>
       </c>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -3152,16 +3120,15 @@
       <c r="I38" t="s">
         <v>189</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="4">
         <v>2.8400000000000002E-2</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="4">
         <f t="shared" si="1"/>
         <v>0.11360000000000001</v>
       </c>
-      <c r="L38"/>
-    </row>
-    <row r="39" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -3189,16 +3156,15 @@
       <c r="I39" t="s">
         <v>192</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="4">
         <v>2.8299999999999999E-2</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="4">
         <f t="shared" si="1"/>
         <v>0.14149999999999999</v>
       </c>
-      <c r="L39"/>
-    </row>
-    <row r="40" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -3226,16 +3192,15 @@
       <c r="I40" t="s">
         <v>194</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="4">
         <v>2.8400000000000002E-2</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="4">
         <f t="shared" si="1"/>
         <v>0.11360000000000001</v>
       </c>
-      <c r="L40"/>
-    </row>
-    <row r="41" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3263,16 +3228,15 @@
       <c r="I41" t="s">
         <v>199</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="4">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="4">
         <f t="shared" si="1"/>
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="L41"/>
-    </row>
-    <row r="42" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>197</v>
       </c>
@@ -3300,16 +3264,15 @@
       <c r="I42" t="s">
         <v>198</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="4">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="4">
         <f t="shared" si="1"/>
         <v>0.31679999999999997</v>
       </c>
-      <c r="L42"/>
-    </row>
-    <row r="43" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -3337,16 +3300,15 @@
       <c r="I43" t="s">
         <v>236</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="4">
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="4">
         <f t="shared" si="1"/>
         <v>2.8799999999999999E-2</v>
       </c>
-      <c r="L43"/>
-    </row>
-    <row r="44" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -3374,16 +3336,15 @@
       <c r="I44" t="s">
         <v>206</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="4">
         <v>1.5</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="L44"/>
-    </row>
-    <row r="45" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>178</v>
       </c>
@@ -3411,16 +3372,15 @@
       <c r="I45" t="s">
         <v>213</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="4">
         <v>1.4</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="4">
         <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
-      <c r="L45"/>
-    </row>
-    <row r="46" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>196</v>
       </c>
@@ -3448,16 +3408,15 @@
       <c r="I46" t="s">
         <v>209</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="4">
         <v>1.25</v>
       </c>
-      <c r="K46">
+      <c r="K46" s="4">
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
-      <c r="L46"/>
-    </row>
-    <row r="47" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -3485,16 +3444,15 @@
       <c r="I47" t="s">
         <v>218</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="4">
         <v>0.90500000000000003</v>
       </c>
-      <c r="K47">
+      <c r="K47" s="4">
         <f t="shared" si="1"/>
         <v>5.43</v>
       </c>
-      <c r="L47"/>
-    </row>
-    <row r="48" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -3522,16 +3480,15 @@
       <c r="I48" t="s">
         <v>222</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="4">
         <v>1.84</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="4">
         <f t="shared" si="1"/>
         <v>1.84</v>
       </c>
-      <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -3559,16 +3516,15 @@
       <c r="I49" t="s">
         <v>226</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="4">
         <v>0.46</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="4">
         <f t="shared" si="1"/>
         <v>0.46</v>
       </c>
-      <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -3596,20 +3552,23 @@
       <c r="I50" t="s">
         <v>229</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="4">
         <v>0.40400000000000003</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="4">
         <f t="shared" si="1"/>
         <v>0.40400000000000003</v>
       </c>
-      <c r="L50"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I51"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I52"/>
       <c r="J52" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="5">
         <f>SUM(K2:K50)</f>
         <v>29.650200000000002</v>
       </c>

</xml_diff>